<commit_message>
update p1 after 1st review
</commit_message>
<xml_diff>
--- a/P1_Report/stroopdata.xlsx
+++ b/P1_Report/stroopdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\Udacity\P1_Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\Udacity\myPro\P1_Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,6 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$25</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$25</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Congruent</t>
   </si>
@@ -40,19 +39,7 @@
     <t>Median</t>
   </si>
   <si>
-    <t>df:c</t>
-  </si>
-  <si>
-    <t>df:i</t>
-  </si>
-  <si>
     <t>mean diff:</t>
-  </si>
-  <si>
-    <t>sem:c</t>
-  </si>
-  <si>
-    <t>sem:i</t>
   </si>
   <si>
     <t>sem:</t>
@@ -64,7 +51,7 @@
     <t>df:</t>
   </si>
   <si>
-    <t>r^2:</t>
+    <t>SD</t>
   </si>
 </sst>
 </file>
@@ -754,16 +741,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -799,7 +786,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4419600" y="762000"/>
+              <a:off x="5572125" y="457200"/>
               <a:ext cx="5210175" cy="2905125"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1130,18 +1117,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1149,260 +1137,432 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12.079000000000001</v>
       </c>
       <c r="B2">
         <v>19.277999999999999</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
+      <c r="C2">
+        <f>B2-A2</f>
+        <v>7.1989999999999981</v>
+      </c>
+      <c r="D2">
+        <f>(C2-$C$27)^2</f>
+        <v>0.58643687673611011</v>
       </c>
       <c r="E2">
-        <f>24-1</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <f>SUM(D2:D25)/23</f>
+        <v>23.666540867753621</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>16.791</v>
       </c>
       <c r="B3">
         <v>18.741</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
+      <c r="C3">
+        <f t="shared" ref="C3:C25" si="0">B3-A3</f>
+        <v>1.9499999999999993</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D25" si="1">(C3-$C$27)^2</f>
+        <v>36.177718793402754</v>
       </c>
       <c r="E3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <f>SQRT(E2)</f>
+        <v>4.8648269103590538</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9.5640000000000001</v>
       </c>
       <c r="B4">
         <v>21.213999999999999</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>11.649999999999999</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>13.580760460069452</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8.6300000000000008</v>
       </c>
       <c r="B5">
         <v>15.686999999999999</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>7.0569999999999986</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>0.8240857100694422</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5">
         <f>B27-A27</f>
         <v>7.9647916666666685</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14.669</v>
       </c>
       <c r="B6">
         <v>22.803000000000001</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <f>A28^2/24</f>
-        <v>0.52787621127717155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>8.1340000000000003</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>2.8631460069445447E-2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>4.8647999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12.238</v>
       </c>
       <c r="B7">
         <v>20.878</v>
       </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <f>B28^2/24</f>
-        <v>0.95882320984299474</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>8.64</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0.4559062934027821</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <f>4.8648/SQRT(24)</f>
+        <v>0.9930231417243004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>14.692</v>
       </c>
       <c r="B8">
         <v>24.571999999999999</v>
       </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <f>SQRT(E6+E7)</f>
-        <v>1.2193028422505077</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>9.879999999999999</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>3.6680229600694507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8.9870000000000001</v>
       </c>
       <c r="B9">
         <v>17.393999999999998</v>
       </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9">
-        <f>E5/E8</f>
-        <v>6.5322505539032356</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>8.4069999999999983</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0.1955482100694452</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <f>G5*SQRT(24)/G6</f>
+        <v>8.0207513118339655</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9.4009999999999998</v>
       </c>
       <c r="B10">
         <v>20.762</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>11.361000000000001</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>11.5342310434028</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>14.48</v>
       </c>
       <c r="B11">
         <v>26.282</v>
       </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11">
-        <f>E9^2/(E9^2+46)</f>
-        <v>0.48122424981950762</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>11.802</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>14.724167793402795</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>22.327999999999999</v>
       </c>
       <c r="B12">
         <v>24.524000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>2.1960000000000015</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>33.278957293402733</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15.298</v>
       </c>
       <c r="B13">
         <v>18.643999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>3.3459999999999983</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>21.333236460069436</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15.073</v>
       </c>
       <c r="B14">
         <v>17.510000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>2.4370000000000012</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>30.556480710069401</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>16.928999999999998</v>
       </c>
       <c r="B15">
         <v>20.329999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>3.4009999999999998</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>20.828194376736089</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>18.2</v>
       </c>
       <c r="B16">
         <v>35.255000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>17.055000000000003</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>82.631887543402897</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12.13</v>
       </c>
       <c r="B17">
         <v>22.158000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>10.028</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>4.2568286267361239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18.495000000000001</v>
       </c>
       <c r="B18">
         <v>25.138999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>6.6439999999999984</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>1.7444906267361087</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10.638999999999999</v>
       </c>
       <c r="B19">
         <v>20.428999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>3.331385460069451</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11.343999999999999</v>
       </c>
       <c r="B20">
         <v>17.425000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>6.0810000000000013</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>3.5486710434027628</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12.369</v>
       </c>
       <c r="B21">
         <v>34.287999999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>21.918999999999997</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>194.71993021006946</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12.944000000000001</v>
       </c>
       <c r="B22">
         <v>23.893999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>10.949999999999998</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>8.9114687934027792</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>14.233000000000001</v>
       </c>
       <c r="B23">
         <v>17.96</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>3.7270000000000003</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>17.958878210069418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>19.71</v>
       </c>
       <c r="B24">
         <v>22.058</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>2.347999999999999</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>31.548348626736093</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>16.004000000000001</v>
       </c>
       <c r="B25">
         <v>21.157</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>5.1529999999999987</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>7.9061723767361034</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>AVERAGE(A2:A25)</f>
         <v>14.051125000000001</v>
@@ -1411,8 +1571,12 @@
         <f>AVERAGE(B2:B25)</f>
         <v>22.015916666666669</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <f>AVERAGE(C2:C25)</f>
+        <v>7.964791666666664</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>_xlfn.STDEV.S(A2:A25)</f>
         <v>3.559357957645187</v>
@@ -1420,6 +1584,10 @@
       <c r="B28">
         <f>_xlfn.STDEV.S(B2:B25)</f>
         <v>4.7970571224691367</v>
+      </c>
+      <c r="C28">
+        <f>_xlfn.STDEV.S(C2:C25)</f>
+        <v>4.8648269103590565</v>
       </c>
     </row>
   </sheetData>
@@ -1432,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>